<commit_message>
Setting map to better latitude
</commit_message>
<xml_diff>
--- a/albums.xlsx
+++ b/albums.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-480" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5786" uniqueCount="5768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6015" uniqueCount="5997">
   <si>
     <r>
       <t xml:space="preserve">1 </t>
@@ -17443,6 +17443,693 @@
   </si>
   <si>
     <t>268 Inside Llewyn Davis:Original Soundtrack Recording-Soundtrack-January            34</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 21-ADELE-MAY                                       5140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  2 SIGH NO MORE-MUMFORD &amp; SONS-February                               1270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  3 SPEAK NOW-TAYLOR SWIFT-January                                                               960</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  4 TAKE CARE-DRAKE-November                                                                     896</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  5 TAILGATES &amp; TANLINES-LUKE BRYAN-August                                         892</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  6 PINK FRIDAY-NICKI MINAJ-February                                                             796</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  7 OWN THE NIGHT-LADY ANTEBELLUM-September                          740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  8 BORN THIS WAY-Lady GaGa-June                                                                 644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  9 MYLO XYLOTO-Coldplay-November                                                                640</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10 TALK THAT TALK-Rihanna-November                                                              608</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11 Tha Carter IV-Lil Wayne-September                                                            568</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12 Christmas-Michael Buble-December                                                             568</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13 El Camino-The Black Keys-December                                                            566</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14 4-Beyonce-July                                                                               566</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15 Clear As Day-Scotty McCreery-October                                                         540</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16 Watch The Throne-Kanye West &amp; Jay-Z-August                                                   502</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17 Hell:The Sequel-Eminem &amp; Royce Da 5'9-June                        448</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18 Never Say Never:The Remixes-Justin Bieber-March                                              444</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19 Under The Mistletoe-Justin Bieber-November                                                   440</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20 Now 40-Various Artists-November                                                              428</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21 Now 38-Various Artists-May                                                                   422</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22 Now 37-Various Artists-February                                                              420</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23 Here And Now-Nickelback-November                                                             416</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24 Torches-Foster The People-June                                                               416</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25 Greatest Hits... So Far!!!-P!nk-February                                                     394</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26 Chief-Eric Church-August                                                                     340</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27 Duets II-Tony Bennett-October                                                                326</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28 Stronger-Kelly Clarkson-November                                                             316</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29 F.A.M.E.-Chris Brown-April                                                                   312</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 30 Dream With Me-Jackie Evancho-June                                                            290</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 31 Femme Fatale-Britney Spears-April                                                            284</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32 Red River Blue-Blake Shelton-July                                                            276</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33 Concerto:One Night In Central Park-Andrea Bocelli-November                                   266</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 34 Wasting Light-Foo Fighters-April                                                             258</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35 Now 39-Various Artists-August                                                                250</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36 Kidz Bop 20-Kidz Bop-August                                                                  240</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 37 Rolling Papers-Wiz Khalifa-April                                                             238</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38 When the Sun Goes Down-Selena Gomez &amp; the Scene-July                                         232</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39 This Is Country Music-Brad Paisley-June                                                      232</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40 Lemonade Mouth Soundtrack-May                                                                212</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41 The Light Of The Sun-Jill Scott-July                                                         204</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42 Cole World:The Sideline Story-Rapper J. Cole-October                                         202</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43 Songs For Japan-Various Artists-April                                                        198</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 44 Ceremonials-Florence + The Machine-November                                                  180</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45 Hello Fear-Kirk Franklin-April                                                               172</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 46 Clancy's Tavern-Toby Keith-November                                                          168</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 47 Lasers-Lupe Fiasco-March                                                                     168</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 48 Evanescence-Evanescence-October                                                              160</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 49 Hot Sauce Committee Part 2-Beastie Boys-May                                                  158</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50 Kidz Bop 19-Kidz Bop-February                                                                152</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 51 I'm With You-Red Hot Chili Peppers-September                                                 150</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 52 I Remember Me-Jennifer Hudson-April                                                          146</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 53 Late Nights &amp; Early Mornings-Marsha Ambrosius-March                                          146</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 54 Tron:Legacy (Soundtrack)-Daft Punk-January                                                   146</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 55 Someone To Watch Over Me-Susan Boyle-November                                                144</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 56 Here For A Good Time-George Strait-September                                                 144</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 57 Helplessness Blues-Fleet Foxes-May                                                           144</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 58 Paper Airplane-Alison Krauss and Union Station-April                                         144</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 59 My Life II...The Journey Continues (Act 1)-Mary J. Blige-November                            142</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 60 So Beautiful Or So What-Paul Simon-April                                                     142</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 61 2011 Grammy Nominees-Various Artists-February                                                142</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 62 Bon Iver-Bon Iver-July                                                                       138</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 63 Love?-Jennifer Lopez-May                                                                     134</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 64 Outlaws Like Me-Justin Moore-July                                                            126</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65 Country Strong Soundtrack-Various Artists-January                                            126</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 66 Glee:The Music:The Christmas Album:Volume 2-Soundtrack-November                              122</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 67 R.E.D.-Game-September                                                                        116</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 68 The King Is Dead-Decemberists-February                                                       112</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 69 Glee TV soundtrack:Volume 5-March                                                            110</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 70 Glee Presents the Warblers-Glee Cast-May                                                     106</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 71 The King of Limbs-Radiohead-April                                                            106</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 72 1-The Beatles-September                                                         (2000)       104</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 73 Turtleneck &amp; Chain-Lonely Island-May                                                         104</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 74 Goodbye Lullaby-Avril Lavigne-March                                                         102</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 75 The Twilight Saga:Breaking Dawn:Part 1-Soundtrack-November                                   100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 76 Come To The Well-Casting Crowns-November                                                     100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 77 American Capitalist-Five Finger Death Punch-October                                          100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 78 Neighborhoods-Blink-182-October                                                              100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 79 Finally Famous-Big Sean-July                                                                 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 80 What Matters Most-Barbra Streisand-September                                                  98</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 81 The Book of Mormon-Original Broadway Cast-June                                                98</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 82 Codes &amp; Keys-Death Cab For Cutie-June                                                         98</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 83 Four The Record-Miranda Lambert-November                                                      96</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 84 Glee,The Music:Season Two,Volume 6-Glee Cast-June                                             96</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 85 Lioness:Hidden Treasures-Amy Winehouse-December                                               94</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 86 Wildflower-Lauren Alaina-November                                                             94</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 87 Ukelele Songs-Eddie Vedder-June                                                               94</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 88 The Whole Love-Wilco-October                                                                  92</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 89 Here I Am-Kelly Rowland-August                                                                92</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 90 Time of My Life-3 Doors Down-August                                                           92</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 91 Back To Black-Amy Winehouse-August                                   (2007)                   92</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 92 If Not Now,When-Incubus-July                                                                  92</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 93 Victorious Soundtrack-August                                                                  90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 94 Neon-Chris Young-July                                                                         90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 95 Maybach Music Group Presents Self Made Vol. 1-Various Artists-June                            90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 96 Best Night Of My Life-Jamie Foxx-January                                                      90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 97 Unbroken-Demi Lovato-October                                                                  88</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 98 Lovestrong-Christina Perri-May                                                                88</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 99 Barefoot Blue Jean Night-Jake Owen-September                                                  86</t>
+  </si>
+  <si>
+    <t>100 We The Best Forever-DJ Khaled-August                                                          86</t>
+  </si>
+  <si>
+    <t>101 Calling All Hearts-Keyshia Cole-January                                                       86</t>
+  </si>
+  <si>
+    <t>102 Planet Pit-Pitbull-July                                                                       82</t>
+  </si>
+  <si>
+    <t>103 Break The Spell-Daughtry-November                                                             80</t>
+  </si>
+  <si>
+    <t>104 Heavenly Christmas-Jackie Evancho-November                                                    74</t>
+  </si>
+  <si>
+    <t>105 Blue Slide Park-Mac Miller-November                                                           70</t>
+  </si>
+  <si>
+    <t>106 Showroom Of Compassion-Cake-January                                                           70</t>
+  </si>
+  <si>
+    <t>107 Mission Bell-Amos Lee-February                                                                70</t>
+  </si>
+  <si>
+    <t>108 Ambition-Wale-November                                                                        58</t>
+  </si>
+  <si>
+    <t>109 Holding Onto To Strings Better Left To Fray-Seether-May                                       58</t>
+  </si>
+  <si>
+    <t>110 Endgame-Rise Against-March                                                                    58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">111 Until We Have Faces-Red-February                                                              58  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">112 Kiss Each Other Clean-Iron and Wine-February                                                  58 </t>
+  </si>
+  <si>
+    <t>113 Thank You Happy Birthday-Cage The Elephant-January                                            58</t>
+  </si>
+  <si>
+    <t>114 Proud to Be Here-Trace Adkins-August                                                          56</t>
+  </si>
+  <si>
+    <t>115 Musica + Alma + Sexo-Ricky Martin-February                                                    56</t>
+  </si>
+  <si>
+    <t>116 Science &amp; Faith-Script-February                                                               56</t>
+  </si>
+  <si>
+    <t>117 Halfway To Heaven-Brantley Gilbert-September                                                  54</t>
+  </si>
+  <si>
+    <t>118 Young Love-Mat Kearney-August                                                                 54</t>
+  </si>
+  <si>
+    <t>119 All 6's &amp; 7's-Tech N9ne-June                                                                  54</t>
+  </si>
+  <si>
+    <t>120 American Tragedy-Hollywood Undead-April                                                       54</t>
+  </si>
+  <si>
+    <t>121 Angles-The Strokes-April                                                                      54</t>
+  </si>
+  <si>
+    <t>122 Hard Times and Nursery Rhymes-Social Distortion-February                                      54</t>
+  </si>
+  <si>
+    <t>123 Staind-Staind-September                                                                       52</t>
+  </si>
+  <si>
+    <t>124 Nothing But The Beat-David Guetta-September                                                   52</t>
+  </si>
+  <si>
+    <t>125 Hell On Heels-Pistol Annies-September                                                         52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">126 Ronnie Dunn-Ronnie Dunn-June                                                                  52 </t>
+  </si>
+  <si>
+    <t>127 Circuital-My Morning Jacket-June                                                              52</t>
+  </si>
+  <si>
+    <t>128 Creator's "Goblin-Tyler-May                                                                   52</t>
+  </si>
+  <si>
+    <t>129 Drama y Luz-Mana-April                                                                        52</t>
+  </si>
+  <si>
+    <t>130 Collapse Into Now-R.E.M-March                                                                 52</t>
+  </si>
+  <si>
+    <t>131 Low Country Blues-Gregg Allman-February                                                       52</t>
+  </si>
+  <si>
+    <t>132 Bad As Me-Tom Waits-October                                                                   50</t>
+  </si>
+  <si>
+    <t>133 The Reckoning-NeedToBreathe-October                                                           50</t>
+  </si>
+  <si>
+    <t>134 Life At Best-Eli Young Band-August                                                            50</t>
+  </si>
+  <si>
+    <t>135 All Of You-Colbie Caillat-July                                                                50</t>
+  </si>
+  <si>
+    <t>136 All Things Bright and Beautiful-Owl City-June                                                 50</t>
+  </si>
+  <si>
+    <t>137 Dirty Work-All Time Low-June                                                                  50</t>
+  </si>
+  <si>
+    <t>138 In Your Dreams-Stevie Nicks-May                                                               50</t>
+  </si>
+  <si>
+    <t>139 Stronger-Sara Evans-March                                                                     50</t>
+  </si>
+  <si>
+    <t>140 Going Out Of Style-Dropkick Murphys-March                                                     50</t>
+  </si>
+  <si>
+    <t>141 Ashes &amp; Fire-Ryan Adams-October                                                               48</t>
+  </si>
+  <si>
+    <t>142 Metals-Feist-October                                                                          48</t>
+  </si>
+  <si>
+    <t>143 #1 Girl-Mindless Behavior-October                                                             48</t>
+  </si>
+  <si>
+    <t>144 Universal Pulse-311-August                                                                    48</t>
+  </si>
+  <si>
+    <t>145 This Loud Morning-David Cook-July                                                             48</t>
+  </si>
+  <si>
+    <t>146 15 Minutes-Barry Manilow-June                                                                 48</t>
+  </si>
+  <si>
+    <t>147 NKOTBSB-New Kids on the Block/Backstreet Boys-June                                            48</t>
+  </si>
+  <si>
+    <t>148 Move Like This-Cars-May                                                                       48</t>
+  </si>
+  <si>
+    <t>149 The Ultimate Collection-Sade-May                                                              48</t>
+  </si>
+  <si>
+    <t>150 Vices &amp; Virtues-Panic At The Disco-April                                                      48</t>
+  </si>
+  <si>
+    <t>151 Town Line-Staind-March                                                                        48</t>
+  </si>
+  <si>
+    <t>152 Steel Magnolia-Steel Magnolia-January                                                         48</t>
+  </si>
+  <si>
+    <t>153 The Good,The Bad,The Sexy-Joe-November                                                        46</t>
+  </si>
+  <si>
+    <t>154 Take A Back Road-Rodney Atkins-October                                                        46</t>
+  </si>
+  <si>
+    <t>155 Vice Verses-Switchfoot-October                                                                46</t>
+  </si>
+  <si>
+    <t>156 Sweeter-Gavin DeGraw-October                                                                  46</t>
+  </si>
+  <si>
+    <t>157 A Dramatic Turn Of Events-Dream Theater-September                                             46</t>
+  </si>
+  <si>
+    <t>158 Muppets:The Green Album-Muppets-September                                                     46</t>
+  </si>
+  <si>
+    <t>159 Any Man in America-Blue October-August                                                        46</t>
+  </si>
+  <si>
+    <t>160 Blood Sweat + Tears-Ace Hood-August                                                           46</t>
+  </si>
+  <si>
+    <t>161 The Truth Is...-Theory of a Deadman-July                                                      46</t>
+  </si>
+  <si>
+    <t>162 Pieces of Me-Ledisi-June                                                                      46</t>
+  </si>
+  <si>
+    <t>163 MusiqInTheMagiq-Musiq Soulchild-May                                                           46</t>
+  </si>
+  <si>
+    <t>164 Doggumentary-Snoop Dogg-April                                                                 46</t>
+  </si>
+  <si>
+    <t>165 Los Vaqueros: El Regreso-Wisin &amp; Yandel-February                                              46</t>
+  </si>
+  <si>
+    <t>166 Glee:The Music:Season 3:Volume 7-Soundtrack-December                                          44</t>
+  </si>
+  <si>
+    <t>167 Formula: Vol. 1-Romeo Santos-November                                                         44</t>
+  </si>
+  <si>
+    <t>168 Open Invitation-Tyrese-November                                                               44</t>
+  </si>
+  <si>
+    <t>169 People and Things-Jack's Mannequin-October                                                    44</t>
+  </si>
+  <si>
+    <t>170 Chickenfoot III-Chickenfoot-October                                                           44</t>
+  </si>
+  <si>
+    <t>171 Slow Grind-Various Artists-August                                                             44</t>
+  </si>
+  <si>
+    <t>172 LP1-Joss Stone-August                                                                         44</t>
+  </si>
+  <si>
+    <t>173 Yours Truly-Rome-July                                                                         44</t>
+  </si>
+  <si>
+    <t>174 Alpocalypse-Weird Al Yankovic-July                                                            44</t>
+  </si>
+  <si>
+    <t>175 Speed of Darkness-Flogging Molly-June                                                         44</t>
+  </si>
+  <si>
+    <t>176 Reckless &amp; Relentless-Asking Alexandria-April                                                 44</t>
+  </si>
+  <si>
+    <t>177 Fly On the Wall-Bobby V-April                                                                 44</t>
+  </si>
+  <si>
+    <t>178 Give The Drummer Some-Sara Evans-March                                                        44</t>
+  </si>
+  <si>
+    <t>179 The Path Of Totality-Korn-December                                                            42</t>
+  </si>
+  <si>
+    <t>180 Wicked Game-Il Divo-November                                                                  42</t>
+  </si>
+  <si>
+    <t>181 Eleven-Martina McBride-October                                                                42</t>
+  </si>
+  <si>
+    <t>182 The Hunter-Mastodon-October                                                                   42</t>
+  </si>
+  <si>
+    <t>183 Pearl Jam Twenty-Pearl Jam-October                                                            42</t>
+  </si>
+  <si>
+    <t>184 Dead Throne-The Devil Wears Prada-September                                                   42</t>
+  </si>
+  <si>
+    <t>185 King Of Hearts-Lloyd-July                                                                     42</t>
+  </si>
+  <si>
+    <t>186 American Idol Season 10 Highlights-Scotty McCreery-July                                       42</t>
+  </si>
+  <si>
+    <t>187 Il Volo-Il Volo-May                                                                           42</t>
+  </si>
+  <si>
+    <t>188 This Is Gonna Hurt-Sixx: A.M.-May                                                             42</t>
+  </si>
+  <si>
+    <t>189 Something Big-Mary Mary-April                                                                 42</t>
+  </si>
+  <si>
+    <t>190 Speak Now: World Tour Live CD + DVD-Taylor Swift-November                                     40</t>
+  </si>
+  <si>
+    <t>191 Camp-Childish Gambino-November                                                                40</t>
+  </si>
+  <si>
+    <t>192 Th1rt3en-Megadeth-November                                                                    40</t>
+  </si>
+  <si>
+    <t>193 Leveler-August Burns Red-July                                                                 40</t>
+  </si>
+  <si>
+    <t>194 Rome-Danger Mouse,Daniele Luppi,Jack White &amp; Norah Jones-May                                  40</t>
+  </si>
+  <si>
+    <t>195 Rumours-Fleetwood Mac-May                                           (1977)                    40</t>
+  </si>
+  <si>
+    <t>196 Who You Are-Jessie J-April                                                                    40</t>
+  </si>
+  <si>
+    <t>197 Heritage-Celtic Thunder-March                                                                 40</t>
+  </si>
+  <si>
+    <t>198 Passion:Here For You-Passion Band-March                                                       40</t>
+  </si>
+  <si>
+    <t>199 Some Kind of Trouble-James Blunt-February                                                     40</t>
+  </si>
+  <si>
+    <t>200 No Boys Allowed-Keri Hilson-January                                                           40</t>
+  </si>
+  <si>
+    <t>201 Back To Love-Anthony Hamilton-December                                                        38</t>
+  </si>
+  <si>
+    <t>202 Elevate (Soundtrack)-Big Time Rush-November                                                   38</t>
+  </si>
+  <si>
+    <t>203 Cities 97 Sampler:Live From Studio C:23-Various Artists-November                              38</t>
+  </si>
+  <si>
+    <t>204 A Very She &amp; Him Christmas-She &amp; Him-November                                                 38</t>
+  </si>
+  <si>
+    <t>205 The Great Escape Artist-Jane's Addiction-November                                             38</t>
+  </si>
+  <si>
+    <t>206 Mayday Parade-Mayday Parade-October                                                           38</t>
+  </si>
+  <si>
+    <t>207 Dark Side of the Moon-Pink Floyd-October                                     (1973)           38</t>
+  </si>
+  <si>
+    <t>208 Coast To Coast (EP)-Cody Simpson-October                                                      38</t>
+  </si>
+  <si>
+    <t>209 Worship Music-Anthrax-September                                                               38</t>
+  </si>
+  <si>
+    <t>210 King-O.A.R.-August                                                                            38</t>
+  </si>
+  <si>
+    <t>211 Revelator-Tedeschi Trucks Band-June                                                           38</t>
+  </si>
+  <si>
+    <t>212 American Idol Season 10-Scotty McCreery-June                                                  38</t>
+  </si>
+  <si>
+    <t>213 Nine Types of Light-TV On the Radio-April                                                     38</t>
+  </si>
+  <si>
+    <t>214 Shaolin vs. Wu-Tang-Raekwon-March                                                              38</t>
+  </si>
+  <si>
+    <t>215 A Merry Little Christmas (EP...)-Lady Antebellum-January                                      38</t>
+  </si>
+  <si>
+    <t>216 The Lost Children-Disturbed-November                                                          36</t>
+  </si>
+  <si>
+    <t>217 Nevermind-Nirvana-October                                                  (1992)             36</t>
+  </si>
+  <si>
+    <t>218 In Waves-Trivium-August                                                                       36</t>
+  </si>
+  <si>
+    <t>219 Michael Grimm-Michael Grimm-May                                                               36</t>
+  </si>
+  <si>
+    <t>220 Family Sign-Atmosphere-April                                                                  36</t>
+  </si>
+  <si>
+    <t>221 How To Become Clairvoyant-Robbie Robertson-April                                              36</t>
+  </si>
+  <si>
+    <t>222 The People's Key-Bright Eyes-March                                                            36</t>
+  </si>
+  <si>
+    <t>223 Guitar Slinger-Vince Gill-November                                                            34</t>
+  </si>
+  <si>
+    <t>224 Footloose Soundtrack-November                                            (1984)               34</t>
+  </si>
+  <si>
+    <t>225 NOW That's What I Call Country:Volume 4-Various Artists-June                                  34</t>
+  </si>
+  <si>
+    <t>226 Suck It And See-Arctic Monkeys -June                                      34</t>
+  </si>
+  <si>
+    <t>227 Stone Rollin'-Raphael Saadiq-May                                                              34</t>
+  </si>
+  <si>
+    <t>228 Awesome As F**k-Green Day-April                                                               34</t>
+  </si>
+  <si>
+    <t>229 Live Forever:September 23,1980-Bob Marley And The Wailers-February                            34</t>
   </si>
 </sst>
 </file>
@@ -17859,13 +18546,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BJ270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BH2" sqref="BH2:BH270"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BE2" sqref="BE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="8" width="10.83203125" customWidth="1"/>
+    <col min="55" max="55" width="27" customWidth="1"/>
+    <col min="57" max="57" width="82.83203125" customWidth="1"/>
+    <col min="58" max="58" width="72.83203125" customWidth="1"/>
+    <col min="59" max="59" width="80.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:62">
@@ -18225,6 +18916,9 @@
       <c r="BD2" t="s">
         <v>4799</v>
       </c>
+      <c r="BE2" t="s">
+        <v>5768</v>
+      </c>
       <c r="BF2" t="s">
         <v>5018</v>
       </c>
@@ -18404,6 +19098,9 @@
       <c r="BD3" t="s">
         <v>4800</v>
       </c>
+      <c r="BE3" t="s">
+        <v>5769</v>
+      </c>
       <c r="BF3" t="s">
         <v>5019</v>
       </c>
@@ -18583,6 +19280,9 @@
       <c r="BD4" t="s">
         <v>4801</v>
       </c>
+      <c r="BE4" t="s">
+        <v>5770</v>
+      </c>
       <c r="BF4" t="s">
         <v>5020</v>
       </c>
@@ -18762,6 +19462,9 @@
       <c r="BD5" t="s">
         <v>4802</v>
       </c>
+      <c r="BE5" t="s">
+        <v>5771</v>
+      </c>
       <c r="BF5" t="s">
         <v>5021</v>
       </c>
@@ -18941,6 +19644,9 @@
       <c r="BD6" t="s">
         <v>4803</v>
       </c>
+      <c r="BE6" t="s">
+        <v>5772</v>
+      </c>
       <c r="BF6" t="s">
         <v>5022</v>
       </c>
@@ -19120,6 +19826,9 @@
       <c r="BD7" t="s">
         <v>4804</v>
       </c>
+      <c r="BE7" t="s">
+        <v>5773</v>
+      </c>
       <c r="BF7" t="s">
         <v>5023</v>
       </c>
@@ -19299,6 +20008,9 @@
       <c r="BD8" t="s">
         <v>4805</v>
       </c>
+      <c r="BE8" t="s">
+        <v>5774</v>
+      </c>
       <c r="BF8" t="s">
         <v>5024</v>
       </c>
@@ -19478,6 +20190,9 @@
       <c r="BD9" t="s">
         <v>4806</v>
       </c>
+      <c r="BE9" t="s">
+        <v>5775</v>
+      </c>
       <c r="BF9" t="s">
         <v>5025</v>
       </c>
@@ -19657,6 +20372,9 @@
       <c r="BD10" t="s">
         <v>4807</v>
       </c>
+      <c r="BE10" t="s">
+        <v>5776</v>
+      </c>
       <c r="BF10" t="s">
         <v>5026</v>
       </c>
@@ -19836,6 +20554,9 @@
       <c r="BD11" t="s">
         <v>4808</v>
       </c>
+      <c r="BE11" t="s">
+        <v>5777</v>
+      </c>
       <c r="BF11" t="s">
         <v>5027</v>
       </c>
@@ -20015,6 +20736,9 @@
       <c r="BD12" t="s">
         <v>4809</v>
       </c>
+      <c r="BE12" t="s">
+        <v>5778</v>
+      </c>
       <c r="BF12" t="s">
         <v>5028</v>
       </c>
@@ -20194,6 +20918,9 @@
       <c r="BD13" t="s">
         <v>4810</v>
       </c>
+      <c r="BE13" t="s">
+        <v>5779</v>
+      </c>
       <c r="BF13" t="s">
         <v>5029</v>
       </c>
@@ -20373,6 +21100,9 @@
       <c r="BD14" t="s">
         <v>4811</v>
       </c>
+      <c r="BE14" t="s">
+        <v>5780</v>
+      </c>
       <c r="BF14" t="s">
         <v>5030</v>
       </c>
@@ -20552,6 +21282,9 @@
       <c r="BD15" t="s">
         <v>4812</v>
       </c>
+      <c r="BE15" t="s">
+        <v>5781</v>
+      </c>
       <c r="BF15" t="s">
         <v>5031</v>
       </c>
@@ -20731,6 +21464,9 @@
       <c r="BD16" t="s">
         <v>4813</v>
       </c>
+      <c r="BE16" t="s">
+        <v>5782</v>
+      </c>
       <c r="BF16" t="s">
         <v>5032</v>
       </c>
@@ -20910,6 +21646,9 @@
       <c r="BD17" t="s">
         <v>4814</v>
       </c>
+      <c r="BE17" t="s">
+        <v>5783</v>
+      </c>
       <c r="BF17" t="s">
         <v>5033</v>
       </c>
@@ -21089,6 +21828,9 @@
       <c r="BD18" t="s">
         <v>4815</v>
       </c>
+      <c r="BE18" t="s">
+        <v>5784</v>
+      </c>
       <c r="BF18" t="s">
         <v>5034</v>
       </c>
@@ -21268,6 +22010,9 @@
       <c r="BD19" t="s">
         <v>4816</v>
       </c>
+      <c r="BE19" t="s">
+        <v>5785</v>
+      </c>
       <c r="BF19" t="s">
         <v>5035</v>
       </c>
@@ -21447,6 +22192,9 @@
       <c r="BD20" t="s">
         <v>4817</v>
       </c>
+      <c r="BE20" t="s">
+        <v>5786</v>
+      </c>
       <c r="BF20" t="s">
         <v>5036</v>
       </c>
@@ -21626,6 +22374,9 @@
       <c r="BD21" t="s">
         <v>4818</v>
       </c>
+      <c r="BE21" t="s">
+        <v>5787</v>
+      </c>
       <c r="BF21" t="s">
         <v>5037</v>
       </c>
@@ -21805,6 +22556,9 @@
       <c r="BD22" t="s">
         <v>4819</v>
       </c>
+      <c r="BE22" t="s">
+        <v>5788</v>
+      </c>
       <c r="BF22" t="s">
         <v>5038</v>
       </c>
@@ -21984,6 +22738,9 @@
       <c r="BD23" t="s">
         <v>4820</v>
       </c>
+      <c r="BE23" t="s">
+        <v>5789</v>
+      </c>
       <c r="BF23" t="s">
         <v>5039</v>
       </c>
@@ -22163,6 +22920,9 @@
       <c r="BD24" t="s">
         <v>4821</v>
       </c>
+      <c r="BE24" t="s">
+        <v>5790</v>
+      </c>
       <c r="BF24" t="s">
         <v>5040</v>
       </c>
@@ -22342,6 +23102,9 @@
       <c r="BD25" t="s">
         <v>4822</v>
       </c>
+      <c r="BE25" t="s">
+        <v>5791</v>
+      </c>
       <c r="BF25" t="s">
         <v>5041</v>
       </c>
@@ -22521,6 +23284,9 @@
       <c r="BD26" t="s">
         <v>4823</v>
       </c>
+      <c r="BE26" t="s">
+        <v>5792</v>
+      </c>
       <c r="BF26" t="s">
         <v>5042</v>
       </c>
@@ -22700,6 +23466,9 @@
       <c r="BD27" t="s">
         <v>4824</v>
       </c>
+      <c r="BE27" t="s">
+        <v>5793</v>
+      </c>
       <c r="BF27" t="s">
         <v>5043</v>
       </c>
@@ -22879,6 +23648,9 @@
       <c r="BD28" t="s">
         <v>4825</v>
       </c>
+      <c r="BE28" t="s">
+        <v>5794</v>
+      </c>
       <c r="BF28" t="s">
         <v>5044</v>
       </c>
@@ -23058,6 +23830,9 @@
       <c r="BD29" t="s">
         <v>4826</v>
       </c>
+      <c r="BE29" t="s">
+        <v>5795</v>
+      </c>
       <c r="BF29" t="s">
         <v>5045</v>
       </c>
@@ -23237,6 +24012,9 @@
       <c r="BD30" t="s">
         <v>4827</v>
       </c>
+      <c r="BE30" t="s">
+        <v>5796</v>
+      </c>
       <c r="BF30" t="s">
         <v>5046</v>
       </c>
@@ -23416,6 +24194,9 @@
       <c r="BD31" t="s">
         <v>4828</v>
       </c>
+      <c r="BE31" t="s">
+        <v>5797</v>
+      </c>
       <c r="BF31" t="s">
         <v>5047</v>
       </c>
@@ -23595,6 +24376,9 @@
       <c r="BD32" t="s">
         <v>4829</v>
       </c>
+      <c r="BE32" t="s">
+        <v>5798</v>
+      </c>
       <c r="BF32" t="s">
         <v>5048</v>
       </c>
@@ -23774,6 +24558,9 @@
       <c r="BD33" t="s">
         <v>4830</v>
       </c>
+      <c r="BE33" t="s">
+        <v>5799</v>
+      </c>
       <c r="BF33" t="s">
         <v>5049</v>
       </c>
@@ -23953,6 +24740,9 @@
       <c r="BD34" t="s">
         <v>4831</v>
       </c>
+      <c r="BE34" t="s">
+        <v>5800</v>
+      </c>
       <c r="BF34" t="s">
         <v>5050</v>
       </c>
@@ -24132,6 +24922,9 @@
       <c r="BD35" t="s">
         <v>4832</v>
       </c>
+      <c r="BE35" t="s">
+        <v>5801</v>
+      </c>
       <c r="BF35" t="s">
         <v>5051</v>
       </c>
@@ -24311,6 +25104,9 @@
       <c r="BD36" t="s">
         <v>4833</v>
       </c>
+      <c r="BE36" t="s">
+        <v>5802</v>
+      </c>
       <c r="BF36" t="s">
         <v>5052</v>
       </c>
@@ -24487,6 +25283,9 @@
       <c r="BD37" t="s">
         <v>4834</v>
       </c>
+      <c r="BE37" t="s">
+        <v>5803</v>
+      </c>
       <c r="BF37" t="s">
         <v>5053</v>
       </c>
@@ -24663,6 +25462,9 @@
       <c r="BD38" t="s">
         <v>4835</v>
       </c>
+      <c r="BE38" t="s">
+        <v>5804</v>
+      </c>
       <c r="BF38" t="s">
         <v>5054</v>
       </c>
@@ -24839,6 +25641,9 @@
       <c r="BD39" t="s">
         <v>4836</v>
       </c>
+      <c r="BE39" t="s">
+        <v>5805</v>
+      </c>
       <c r="BF39" t="s">
         <v>5055</v>
       </c>
@@ -25015,6 +25820,9 @@
       <c r="BD40" t="s">
         <v>4837</v>
       </c>
+      <c r="BE40" t="s">
+        <v>5806</v>
+      </c>
       <c r="BF40" t="s">
         <v>5056</v>
       </c>
@@ -25191,6 +25999,9 @@
       <c r="BD41" t="s">
         <v>4838</v>
       </c>
+      <c r="BE41" t="s">
+        <v>5807</v>
+      </c>
       <c r="BF41" t="s">
         <v>5057</v>
       </c>
@@ -25367,6 +26178,9 @@
       <c r="BD42" t="s">
         <v>4839</v>
       </c>
+      <c r="BE42" t="s">
+        <v>5808</v>
+      </c>
       <c r="BF42" t="s">
         <v>5058</v>
       </c>
@@ -25543,6 +26357,9 @@
       <c r="BD43" t="s">
         <v>4840</v>
       </c>
+      <c r="BE43" t="s">
+        <v>5809</v>
+      </c>
       <c r="BF43" t="s">
         <v>5059</v>
       </c>
@@ -25719,6 +26536,9 @@
       <c r="BD44" t="s">
         <v>4841</v>
       </c>
+      <c r="BE44" t="s">
+        <v>5810</v>
+      </c>
       <c r="BF44" t="s">
         <v>5060</v>
       </c>
@@ -25892,6 +26712,9 @@
       <c r="BD45" t="s">
         <v>4842</v>
       </c>
+      <c r="BE45" t="s">
+        <v>5811</v>
+      </c>
       <c r="BF45" t="s">
         <v>5061</v>
       </c>
@@ -26056,6 +26879,9 @@
       <c r="BD46" t="s">
         <v>4843</v>
       </c>
+      <c r="BE46" t="s">
+        <v>5812</v>
+      </c>
       <c r="BF46" t="s">
         <v>5062</v>
       </c>
@@ -26220,6 +27046,9 @@
       <c r="BD47" t="s">
         <v>4844</v>
       </c>
+      <c r="BE47" t="s">
+        <v>5813</v>
+      </c>
       <c r="BF47" t="s">
         <v>5063</v>
       </c>
@@ -26381,6 +27210,9 @@
       <c r="BD48" t="s">
         <v>4845</v>
       </c>
+      <c r="BE48" t="s">
+        <v>5814</v>
+      </c>
       <c r="BF48" t="s">
         <v>5064</v>
       </c>
@@ -26539,6 +27371,9 @@
       <c r="BD49" t="s">
         <v>4846</v>
       </c>
+      <c r="BE49" t="s">
+        <v>5815</v>
+      </c>
       <c r="BF49" t="s">
         <v>5065</v>
       </c>
@@ -26691,6 +27526,9 @@
       <c r="BD50" t="s">
         <v>4847</v>
       </c>
+      <c r="BE50" t="s">
+        <v>5816</v>
+      </c>
       <c r="BF50" t="s">
         <v>5066</v>
       </c>
@@ -26840,6 +27678,9 @@
       <c r="BD51" t="s">
         <v>4848</v>
       </c>
+      <c r="BE51" t="s">
+        <v>5817</v>
+      </c>
       <c r="BF51" t="s">
         <v>5067</v>
       </c>
@@ -26989,6 +27830,9 @@
       <c r="BD52" t="s">
         <v>4849</v>
       </c>
+      <c r="BE52" t="s">
+        <v>5818</v>
+      </c>
       <c r="BF52" t="s">
         <v>5068</v>
       </c>
@@ -27132,6 +27976,9 @@
       <c r="BD53" t="s">
         <v>4850</v>
       </c>
+      <c r="BE53" t="s">
+        <v>5819</v>
+      </c>
       <c r="BF53" t="s">
         <v>5069</v>
       </c>
@@ -27275,6 +28122,9 @@
       <c r="BD54" t="s">
         <v>4851</v>
       </c>
+      <c r="BE54" t="s">
+        <v>5820</v>
+      </c>
       <c r="BF54" t="s">
         <v>5070</v>
       </c>
@@ -27418,6 +28268,9 @@
       <c r="BD55" t="s">
         <v>4852</v>
       </c>
+      <c r="BE55" t="s">
+        <v>5821</v>
+      </c>
       <c r="BF55" t="s">
         <v>5071</v>
       </c>
@@ -27561,6 +28414,9 @@
       <c r="BD56" t="s">
         <v>4853</v>
       </c>
+      <c r="BE56" t="s">
+        <v>5822</v>
+      </c>
       <c r="BF56" t="s">
         <v>5072</v>
       </c>
@@ -27701,6 +28557,9 @@
       <c r="BD57" t="s">
         <v>4854</v>
       </c>
+      <c r="BE57" t="s">
+        <v>5823</v>
+      </c>
       <c r="BF57" t="s">
         <v>5073</v>
       </c>
@@ -27835,6 +28694,9 @@
       <c r="BD58" t="s">
         <v>4855</v>
       </c>
+      <c r="BE58" t="s">
+        <v>5824</v>
+      </c>
       <c r="BF58" t="s">
         <v>5074</v>
       </c>
@@ -27969,6 +28831,9 @@
       <c r="BD59" t="s">
         <v>4856</v>
       </c>
+      <c r="BE59" t="s">
+        <v>5825</v>
+      </c>
       <c r="BF59" t="s">
         <v>5075</v>
       </c>
@@ -28100,6 +28965,9 @@
       <c r="BD60" t="s">
         <v>4857</v>
       </c>
+      <c r="BE60" t="s">
+        <v>5826</v>
+      </c>
       <c r="BF60" t="s">
         <v>5076</v>
       </c>
@@ -28225,6 +29093,9 @@
       <c r="BD61" t="s">
         <v>4858</v>
       </c>
+      <c r="BE61" t="s">
+        <v>5827</v>
+      </c>
       <c r="BF61" t="s">
         <v>5077</v>
       </c>
@@ -28350,6 +29221,9 @@
       <c r="BD62" t="s">
         <v>4859</v>
       </c>
+      <c r="BE62" t="s">
+        <v>5828</v>
+      </c>
       <c r="BF62" t="s">
         <v>5078</v>
       </c>
@@ -28463,6 +29337,9 @@
       <c r="BD63" t="s">
         <v>4860</v>
       </c>
+      <c r="BE63" t="s">
+        <v>5829</v>
+      </c>
       <c r="BF63" t="s">
         <v>5079</v>
       </c>
@@ -28573,6 +29450,9 @@
       <c r="BD64" t="s">
         <v>4861</v>
       </c>
+      <c r="BE64" t="s">
+        <v>5830</v>
+      </c>
       <c r="BF64" t="s">
         <v>5080</v>
       </c>
@@ -28677,6 +29557,9 @@
       <c r="BD65" t="s">
         <v>4862</v>
       </c>
+      <c r="BE65" t="s">
+        <v>5831</v>
+      </c>
       <c r="BF65" t="s">
         <v>5081</v>
       </c>
@@ -28775,6 +29658,9 @@
       <c r="BD66" t="s">
         <v>4863</v>
       </c>
+      <c r="BE66" t="s">
+        <v>5832</v>
+      </c>
       <c r="BF66" t="s">
         <v>5082</v>
       </c>
@@ -28873,6 +29759,9 @@
       <c r="BD67" t="s">
         <v>4864</v>
       </c>
+      <c r="BE67" t="s">
+        <v>5833</v>
+      </c>
       <c r="BF67" t="s">
         <v>5083</v>
       </c>
@@ -28971,6 +29860,9 @@
       <c r="BD68" t="s">
         <v>4865</v>
       </c>
+      <c r="BE68" t="s">
+        <v>5834</v>
+      </c>
       <c r="BF68" t="s">
         <v>5084</v>
       </c>
@@ -29066,6 +29958,9 @@
       <c r="BD69" t="s">
         <v>4866</v>
       </c>
+      <c r="BE69" t="s">
+        <v>5835</v>
+      </c>
       <c r="BF69" t="s">
         <v>5085</v>
       </c>
@@ -29161,6 +30056,9 @@
       <c r="BD70" t="s">
         <v>4867</v>
       </c>
+      <c r="BE70" t="s">
+        <v>5836</v>
+      </c>
       <c r="BF70" t="s">
         <v>5086</v>
       </c>
@@ -29253,6 +30151,9 @@
       <c r="BD71" t="s">
         <v>4868</v>
       </c>
+      <c r="BE71" t="s">
+        <v>5837</v>
+      </c>
       <c r="BF71" t="s">
         <v>5087</v>
       </c>
@@ -29345,6 +30246,9 @@
       <c r="BD72" t="s">
         <v>4869</v>
       </c>
+      <c r="BE72" t="s">
+        <v>5838</v>
+      </c>
       <c r="BF72" t="s">
         <v>5088</v>
       </c>
@@ -29437,6 +30341,9 @@
       <c r="BD73" t="s">
         <v>4870</v>
       </c>
+      <c r="BE73" t="s">
+        <v>5839</v>
+      </c>
       <c r="BF73" t="s">
         <v>5089</v>
       </c>
@@ -29529,6 +30436,9 @@
       <c r="BD74" t="s">
         <v>4871</v>
       </c>
+      <c r="BE74" t="s">
+        <v>5840</v>
+      </c>
       <c r="BF74" t="s">
         <v>5090</v>
       </c>
@@ -29615,6 +30525,9 @@
       <c r="BD75" t="s">
         <v>4872</v>
       </c>
+      <c r="BE75" t="s">
+        <v>5841</v>
+      </c>
       <c r="BF75" t="s">
         <v>5091</v>
       </c>
@@ -29701,6 +30614,9 @@
       <c r="BD76" t="s">
         <v>4873</v>
       </c>
+      <c r="BE76" t="s">
+        <v>5842</v>
+      </c>
       <c r="BF76" t="s">
         <v>5092</v>
       </c>
@@ -29781,6 +30697,9 @@
       <c r="BD77" t="s">
         <v>4874</v>
       </c>
+      <c r="BE77" t="s">
+        <v>5843</v>
+      </c>
       <c r="BF77" t="s">
         <v>5093</v>
       </c>
@@ -29861,6 +30780,9 @@
       <c r="BD78" t="s">
         <v>4875</v>
       </c>
+      <c r="BE78" t="s">
+        <v>5844</v>
+      </c>
       <c r="BF78" t="s">
         <v>5094</v>
       </c>
@@ -29941,6 +30863,9 @@
       <c r="BD79" t="s">
         <v>4876</v>
       </c>
+      <c r="BE79" t="s">
+        <v>5845</v>
+      </c>
       <c r="BF79" t="s">
         <v>5095</v>
       </c>
@@ -30021,6 +30946,9 @@
       <c r="BD80" t="s">
         <v>4877</v>
       </c>
+      <c r="BE80" t="s">
+        <v>5846</v>
+      </c>
       <c r="BF80" t="s">
         <v>5096</v>
       </c>
@@ -30101,6 +31029,9 @@
       <c r="BD81" t="s">
         <v>4878</v>
       </c>
+      <c r="BE81" t="s">
+        <v>5847</v>
+      </c>
       <c r="BF81" t="s">
         <v>5097</v>
       </c>
@@ -30178,6 +31109,9 @@
       <c r="BD82" t="s">
         <v>4879</v>
       </c>
+      <c r="BE82" t="s">
+        <v>5848</v>
+      </c>
       <c r="BF82" t="s">
         <v>5098</v>
       </c>
@@ -30255,6 +31189,9 @@
       <c r="BD83" t="s">
         <v>4880</v>
       </c>
+      <c r="BE83" t="s">
+        <v>5849</v>
+      </c>
       <c r="BF83" t="s">
         <v>5099</v>
       </c>
@@ -30329,6 +31266,9 @@
       <c r="BD84" t="s">
         <v>4881</v>
       </c>
+      <c r="BE84" t="s">
+        <v>5850</v>
+      </c>
       <c r="BF84" t="s">
         <v>5100</v>
       </c>
@@ -30397,6 +31337,9 @@
       <c r="BD85" t="s">
         <v>4882</v>
       </c>
+      <c r="BE85" t="s">
+        <v>5851</v>
+      </c>
       <c r="BF85" t="s">
         <v>5101</v>
       </c>
@@ -30465,6 +31408,9 @@
       <c r="BD86" t="s">
         <v>4883</v>
       </c>
+      <c r="BE86" t="s">
+        <v>5852</v>
+      </c>
       <c r="BF86" t="s">
         <v>5102</v>
       </c>
@@ -30533,6 +31479,9 @@
       <c r="BD87" t="s">
         <v>4884</v>
       </c>
+      <c r="BE87" t="s">
+        <v>5853</v>
+      </c>
       <c r="BF87" t="s">
         <v>5103</v>
       </c>
@@ -30601,6 +31550,9 @@
       <c r="BD88" t="s">
         <v>4885</v>
       </c>
+      <c r="BE88" t="s">
+        <v>5854</v>
+      </c>
       <c r="BF88" t="s">
         <v>5104</v>
       </c>
@@ -30669,6 +31621,9 @@
       <c r="BD89" t="s">
         <v>4886</v>
       </c>
+      <c r="BE89" t="s">
+        <v>5855</v>
+      </c>
       <c r="BF89" t="s">
         <v>5105</v>
       </c>
@@ -30737,6 +31692,9 @@
       <c r="BD90" t="s">
         <v>4887</v>
       </c>
+      <c r="BE90" t="s">
+        <v>5856</v>
+      </c>
       <c r="BF90" t="s">
         <v>5106</v>
       </c>
@@ -30805,6 +31763,9 @@
       <c r="BD91" t="s">
         <v>4888</v>
       </c>
+      <c r="BE91" t="s">
+        <v>5857</v>
+      </c>
       <c r="BF91" t="s">
         <v>5107</v>
       </c>
@@ -30873,6 +31834,9 @@
       <c r="BD92" t="s">
         <v>4889</v>
       </c>
+      <c r="BE92" t="s">
+        <v>5858</v>
+      </c>
       <c r="BF92" t="s">
         <v>5108</v>
       </c>
@@ -30938,6 +31902,9 @@
       <c r="BD93" t="s">
         <v>4890</v>
       </c>
+      <c r="BE93" t="s">
+        <v>5859</v>
+      </c>
       <c r="BF93" t="s">
         <v>5109</v>
       </c>
@@ -31000,6 +31967,9 @@
       <c r="BD94" t="s">
         <v>4891</v>
       </c>
+      <c r="BE94" t="s">
+        <v>5860</v>
+      </c>
       <c r="BF94" t="s">
         <v>5110</v>
       </c>
@@ -31056,6 +32026,9 @@
       <c r="BD95" t="s">
         <v>4892</v>
       </c>
+      <c r="BE95" t="s">
+        <v>5861</v>
+      </c>
       <c r="BF95" t="s">
         <v>5111</v>
       </c>
@@ -31112,6 +32085,9 @@
       <c r="BD96" t="s">
         <v>4893</v>
       </c>
+      <c r="BE96" t="s">
+        <v>5862</v>
+      </c>
       <c r="BF96" t="s">
         <v>5112</v>
       </c>
@@ -31168,6 +32144,9 @@
       <c r="BD97" t="s">
         <v>4894</v>
       </c>
+      <c r="BE97" t="s">
+        <v>5863</v>
+      </c>
       <c r="BF97" t="s">
         <v>5113</v>
       </c>
@@ -31221,6 +32200,9 @@
       <c r="BD98" t="s">
         <v>4895</v>
       </c>
+      <c r="BE98" t="s">
+        <v>5864</v>
+      </c>
       <c r="BF98" t="s">
         <v>5114</v>
       </c>
@@ -31274,6 +32256,9 @@
       <c r="BD99" t="s">
         <v>4896</v>
       </c>
+      <c r="BE99" t="s">
+        <v>5865</v>
+      </c>
       <c r="BF99" t="s">
         <v>5115</v>
       </c>
@@ -31327,6 +32312,9 @@
       <c r="BD100" t="s">
         <v>4897</v>
       </c>
+      <c r="BE100" t="s">
+        <v>5866</v>
+      </c>
       <c r="BF100" t="s">
         <v>5116</v>
       </c>
@@ -31380,6 +32368,9 @@
       <c r="BD101" t="s">
         <v>4898</v>
       </c>
+      <c r="BE101" t="s">
+        <v>5867</v>
+      </c>
       <c r="BF101" t="s">
         <v>5117</v>
       </c>
@@ -31433,6 +32424,9 @@
       <c r="BD102" t="s">
         <v>4899</v>
       </c>
+      <c r="BE102" t="s">
+        <v>5868</v>
+      </c>
       <c r="BF102" t="s">
         <v>5118</v>
       </c>
@@ -31486,6 +32480,9 @@
       <c r="BD103" t="s">
         <v>4900</v>
       </c>
+      <c r="BE103" t="s">
+        <v>5869</v>
+      </c>
       <c r="BF103" t="s">
         <v>5119</v>
       </c>
@@ -31536,6 +32533,9 @@
       <c r="BD104" t="s">
         <v>4901</v>
       </c>
+      <c r="BE104" t="s">
+        <v>5870</v>
+      </c>
       <c r="BF104" t="s">
         <v>5120</v>
       </c>
@@ -31586,6 +32586,9 @@
       <c r="BD105" t="s">
         <v>4902</v>
       </c>
+      <c r="BE105" t="s">
+        <v>5871</v>
+      </c>
       <c r="BF105" t="s">
         <v>5121</v>
       </c>
@@ -31636,6 +32639,9 @@
       <c r="BD106" t="s">
         <v>4903</v>
       </c>
+      <c r="BE106" t="s">
+        <v>5872</v>
+      </c>
       <c r="BF106" t="s">
         <v>5122</v>
       </c>
@@ -31686,6 +32692,9 @@
       <c r="BD107" t="s">
         <v>4904</v>
       </c>
+      <c r="BE107" t="s">
+        <v>5873</v>
+      </c>
       <c r="BF107" t="s">
         <v>5123</v>
       </c>
@@ -31736,6 +32745,9 @@
       <c r="BD108" t="s">
         <v>4905</v>
       </c>
+      <c r="BE108" t="s">
+        <v>5874</v>
+      </c>
       <c r="BF108" t="s">
         <v>5124</v>
       </c>
@@ -31786,6 +32798,9 @@
       <c r="BD109" t="s">
         <v>4906</v>
       </c>
+      <c r="BE109" t="s">
+        <v>5875</v>
+      </c>
       <c r="BF109" t="s">
         <v>5125</v>
       </c>
@@ -31836,6 +32851,9 @@
       <c r="BD110" t="s">
         <v>4907</v>
       </c>
+      <c r="BE110" t="s">
+        <v>5876</v>
+      </c>
       <c r="BF110" t="s">
         <v>5126</v>
       </c>
@@ -31886,6 +32904,9 @@
       <c r="BD111" t="s">
         <v>4908</v>
       </c>
+      <c r="BE111" t="s">
+        <v>5877</v>
+      </c>
       <c r="BF111" t="s">
         <v>5127</v>
       </c>
@@ -31936,6 +32957,9 @@
       <c r="BD112" t="s">
         <v>4909</v>
       </c>
+      <c r="BE112" t="s">
+        <v>5878</v>
+      </c>
       <c r="BF112" t="s">
         <v>5128</v>
       </c>
@@ -31986,6 +33010,9 @@
       <c r="BD113" t="s">
         <v>4910</v>
       </c>
+      <c r="BE113" t="s">
+        <v>5879</v>
+      </c>
       <c r="BF113" t="s">
         <v>5129</v>
       </c>
@@ -32036,6 +33063,9 @@
       <c r="BD114" t="s">
         <v>4911</v>
       </c>
+      <c r="BE114" t="s">
+        <v>5880</v>
+      </c>
       <c r="BF114" t="s">
         <v>5130</v>
       </c>
@@ -32083,6 +33113,9 @@
       <c r="BD115" t="s">
         <v>4912</v>
       </c>
+      <c r="BE115" t="s">
+        <v>5881</v>
+      </c>
       <c r="BF115" t="s">
         <v>5131</v>
       </c>
@@ -32130,6 +33163,9 @@
       <c r="BD116" t="s">
         <v>4913</v>
       </c>
+      <c r="BE116" t="s">
+        <v>5882</v>
+      </c>
       <c r="BF116" t="s">
         <v>5132</v>
       </c>
@@ -32177,6 +33213,9 @@
       <c r="BD117" t="s">
         <v>4914</v>
       </c>
+      <c r="BE117" t="s">
+        <v>5883</v>
+      </c>
       <c r="BF117" t="s">
         <v>5133</v>
       </c>
@@ -32224,6 +33263,9 @@
       <c r="BD118" t="s">
         <v>4915</v>
       </c>
+      <c r="BE118" t="s">
+        <v>5884</v>
+      </c>
       <c r="BF118" t="s">
         <v>5134</v>
       </c>
@@ -32271,6 +33313,9 @@
       <c r="BD119" t="s">
         <v>4916</v>
       </c>
+      <c r="BE119" t="s">
+        <v>5885</v>
+      </c>
       <c r="BF119" t="s">
         <v>5135</v>
       </c>
@@ -32318,6 +33363,9 @@
       <c r="BD120" t="s">
         <v>4917</v>
       </c>
+      <c r="BE120" t="s">
+        <v>5886</v>
+      </c>
       <c r="BF120" t="s">
         <v>5136</v>
       </c>
@@ -32362,6 +33410,9 @@
       <c r="BD121" t="s">
         <v>4918</v>
       </c>
+      <c r="BE121" t="s">
+        <v>5887</v>
+      </c>
       <c r="BF121" t="s">
         <v>5137</v>
       </c>
@@ -32406,6 +33457,9 @@
       <c r="BD122" t="s">
         <v>4919</v>
       </c>
+      <c r="BE122" t="s">
+        <v>5888</v>
+      </c>
       <c r="BF122" t="s">
         <v>5138</v>
       </c>
@@ -32450,6 +33504,9 @@
       <c r="BD123" t="s">
         <v>4920</v>
       </c>
+      <c r="BE123" t="s">
+        <v>5889</v>
+      </c>
       <c r="BF123" t="s">
         <v>5139</v>
       </c>
@@ -32494,6 +33551,9 @@
       <c r="BD124" t="s">
         <v>4921</v>
       </c>
+      <c r="BE124" t="s">
+        <v>5890</v>
+      </c>
       <c r="BF124" t="s">
         <v>5140</v>
       </c>
@@ -32538,6 +33598,9 @@
       <c r="BD125" t="s">
         <v>4922</v>
       </c>
+      <c r="BE125" t="s">
+        <v>5891</v>
+      </c>
       <c r="BF125" t="s">
         <v>5141</v>
       </c>
@@ -32579,6 +33642,9 @@
       <c r="BD126" t="s">
         <v>4923</v>
       </c>
+      <c r="BE126" t="s">
+        <v>5892</v>
+      </c>
       <c r="BF126" t="s">
         <v>5142</v>
       </c>
@@ -32620,6 +33686,9 @@
       <c r="BD127" t="s">
         <v>4924</v>
       </c>
+      <c r="BE127" t="s">
+        <v>5893</v>
+      </c>
       <c r="BF127" t="s">
         <v>5143</v>
       </c>
@@ -32661,6 +33730,9 @@
       <c r="BD128" t="s">
         <v>4925</v>
       </c>
+      <c r="BE128" t="s">
+        <v>5894</v>
+      </c>
       <c r="BF128" t="s">
         <v>5144</v>
       </c>
@@ -32702,6 +33774,9 @@
       <c r="BD129" t="s">
         <v>4926</v>
       </c>
+      <c r="BE129" t="s">
+        <v>5895</v>
+      </c>
       <c r="BF129" t="s">
         <v>5145</v>
       </c>
@@ -32743,6 +33818,9 @@
       <c r="BD130" t="s">
         <v>4927</v>
       </c>
+      <c r="BE130" t="s">
+        <v>5896</v>
+      </c>
       <c r="BF130" t="s">
         <v>5146</v>
       </c>
@@ -32784,6 +33862,9 @@
       <c r="BD131" t="s">
         <v>4928</v>
       </c>
+      <c r="BE131" t="s">
+        <v>5897</v>
+      </c>
       <c r="BF131" t="s">
         <v>5147</v>
       </c>
@@ -32825,6 +33906,9 @@
       <c r="BD132" t="s">
         <v>4929</v>
       </c>
+      <c r="BE132" t="s">
+        <v>5898</v>
+      </c>
       <c r="BF132" t="s">
         <v>5148</v>
       </c>
@@ -32866,6 +33950,9 @@
       <c r="BD133" t="s">
         <v>4930</v>
       </c>
+      <c r="BE133" t="s">
+        <v>5899</v>
+      </c>
       <c r="BF133" t="s">
         <v>5149</v>
       </c>
@@ -32907,6 +33994,9 @@
       <c r="BD134" t="s">
         <v>4931</v>
       </c>
+      <c r="BE134" t="s">
+        <v>5900</v>
+      </c>
       <c r="BF134" t="s">
         <v>5150</v>
       </c>
@@ -32948,6 +34038,9 @@
       <c r="BD135" t="s">
         <v>4932</v>
       </c>
+      <c r="BE135" t="s">
+        <v>5901</v>
+      </c>
       <c r="BF135" t="s">
         <v>5151</v>
       </c>
@@ -32989,6 +34082,9 @@
       <c r="BD136" t="s">
         <v>4933</v>
       </c>
+      <c r="BE136" t="s">
+        <v>5902</v>
+      </c>
       <c r="BF136" t="s">
         <v>5152</v>
       </c>
@@ -33030,6 +34126,9 @@
       <c r="BD137" t="s">
         <v>4934</v>
       </c>
+      <c r="BE137" t="s">
+        <v>5903</v>
+      </c>
       <c r="BF137" t="s">
         <v>5153</v>
       </c>
@@ -33071,6 +34170,9 @@
       <c r="BD138" t="s">
         <v>4935</v>
       </c>
+      <c r="BE138" t="s">
+        <v>5904</v>
+      </c>
       <c r="BF138" t="s">
         <v>5154</v>
       </c>
@@ -33112,6 +34214,9 @@
       <c r="BD139" t="s">
         <v>4936</v>
       </c>
+      <c r="BE139" t="s">
+        <v>5905</v>
+      </c>
       <c r="BF139" t="s">
         <v>5155</v>
       </c>
@@ -33153,6 +34258,9 @@
       <c r="BD140" t="s">
         <v>4937</v>
       </c>
+      <c r="BE140" t="s">
+        <v>5906</v>
+      </c>
       <c r="BF140" t="s">
         <v>5156</v>
       </c>
@@ -33194,6 +34302,9 @@
       <c r="BD141" t="s">
         <v>4938</v>
       </c>
+      <c r="BE141" t="s">
+        <v>5907</v>
+      </c>
       <c r="BF141" t="s">
         <v>5157</v>
       </c>
@@ -33235,6 +34346,9 @@
       <c r="BD142" t="s">
         <v>4939</v>
       </c>
+      <c r="BE142" t="s">
+        <v>5908</v>
+      </c>
       <c r="BF142" t="s">
         <v>5158</v>
       </c>
@@ -33276,6 +34390,9 @@
       <c r="BD143" t="s">
         <v>4940</v>
       </c>
+      <c r="BE143" t="s">
+        <v>5909</v>
+      </c>
       <c r="BF143" t="s">
         <v>5159</v>
       </c>
@@ -33317,6 +34434,9 @@
       <c r="BD144" t="s">
         <v>4941</v>
       </c>
+      <c r="BE144" t="s">
+        <v>5910</v>
+      </c>
       <c r="BF144" t="s">
         <v>5160</v>
       </c>
@@ -33358,6 +34478,9 @@
       <c r="BD145" t="s">
         <v>4942</v>
       </c>
+      <c r="BE145" t="s">
+        <v>5911</v>
+      </c>
       <c r="BF145" t="s">
         <v>5161</v>
       </c>
@@ -33399,6 +34522,9 @@
       <c r="BD146" t="s">
         <v>4943</v>
       </c>
+      <c r="BE146" t="s">
+        <v>5912</v>
+      </c>
       <c r="BF146" t="s">
         <v>5162</v>
       </c>
@@ -33440,6 +34566,9 @@
       <c r="BD147" t="s">
         <v>4944</v>
       </c>
+      <c r="BE147" t="s">
+        <v>5913</v>
+      </c>
       <c r="BF147" t="s">
         <v>5163</v>
       </c>
@@ -33478,6 +34607,9 @@
       <c r="BD148" t="s">
         <v>4945</v>
       </c>
+      <c r="BE148" t="s">
+        <v>5914</v>
+      </c>
       <c r="BF148" t="s">
         <v>5164</v>
       </c>
@@ -33516,6 +34648,9 @@
       <c r="BD149" t="s">
         <v>4946</v>
       </c>
+      <c r="BE149" t="s">
+        <v>5915</v>
+      </c>
       <c r="BF149" t="s">
         <v>5165</v>
       </c>
@@ -33554,6 +34689,9 @@
       <c r="BD150" t="s">
         <v>4947</v>
       </c>
+      <c r="BE150" t="s">
+        <v>5916</v>
+      </c>
       <c r="BF150" t="s">
         <v>5166</v>
       </c>
@@ -33592,6 +34730,9 @@
       <c r="BD151" t="s">
         <v>4948</v>
       </c>
+      <c r="BE151" t="s">
+        <v>5917</v>
+      </c>
       <c r="BF151" t="s">
         <v>5167</v>
       </c>
@@ -33630,6 +34771,9 @@
       <c r="BD152" t="s">
         <v>4949</v>
       </c>
+      <c r="BE152" t="s">
+        <v>5918</v>
+      </c>
       <c r="BF152" t="s">
         <v>5168</v>
       </c>
@@ -33668,6 +34812,9 @@
       <c r="BD153" t="s">
         <v>4950</v>
       </c>
+      <c r="BE153" t="s">
+        <v>5919</v>
+      </c>
       <c r="BF153" t="s">
         <v>5169</v>
       </c>
@@ -33706,6 +34853,9 @@
       <c r="BD154" t="s">
         <v>4951</v>
       </c>
+      <c r="BE154" t="s">
+        <v>5920</v>
+      </c>
       <c r="BF154" t="s">
         <v>5170</v>
       </c>
@@ -33744,6 +34894,9 @@
       <c r="BD155" t="s">
         <v>4952</v>
       </c>
+      <c r="BE155" t="s">
+        <v>5921</v>
+      </c>
       <c r="BF155" t="s">
         <v>5171</v>
       </c>
@@ -33782,6 +34935,9 @@
       <c r="BD156" t="s">
         <v>4953</v>
       </c>
+      <c r="BE156" t="s">
+        <v>5922</v>
+      </c>
       <c r="BF156" t="s">
         <v>5172</v>
       </c>
@@ -33820,6 +34976,9 @@
       <c r="BD157" t="s">
         <v>4954</v>
       </c>
+      <c r="BE157" t="s">
+        <v>5923</v>
+      </c>
       <c r="BF157" t="s">
         <v>5173</v>
       </c>
@@ -33858,6 +35017,9 @@
       <c r="BD158" t="s">
         <v>4955</v>
       </c>
+      <c r="BE158" t="s">
+        <v>5924</v>
+      </c>
       <c r="BF158" t="s">
         <v>5174</v>
       </c>
@@ -33896,6 +35058,9 @@
       <c r="BD159" t="s">
         <v>4956</v>
       </c>
+      <c r="BE159" t="s">
+        <v>5925</v>
+      </c>
       <c r="BF159" t="s">
         <v>5175</v>
       </c>
@@ -33934,6 +35099,9 @@
       <c r="BD160" t="s">
         <v>4957</v>
       </c>
+      <c r="BE160" t="s">
+        <v>5926</v>
+      </c>
       <c r="BF160" t="s">
         <v>5176</v>
       </c>
@@ -33972,6 +35140,9 @@
       <c r="BD161" t="s">
         <v>4958</v>
       </c>
+      <c r="BE161" t="s">
+        <v>5927</v>
+      </c>
       <c r="BF161" t="s">
         <v>5177</v>
       </c>
@@ -34010,6 +35181,9 @@
       <c r="BD162" t="s">
         <v>4959</v>
       </c>
+      <c r="BE162" t="s">
+        <v>5928</v>
+      </c>
       <c r="BF162" t="s">
         <v>5178</v>
       </c>
@@ -34048,6 +35222,9 @@
       <c r="BD163" t="s">
         <v>4960</v>
       </c>
+      <c r="BE163" t="s">
+        <v>5929</v>
+      </c>
       <c r="BF163" t="s">
         <v>5179</v>
       </c>
@@ -34086,6 +35263,9 @@
       <c r="BD164" t="s">
         <v>4961</v>
       </c>
+      <c r="BE164" t="s">
+        <v>5930</v>
+      </c>
       <c r="BF164" t="s">
         <v>5180</v>
       </c>
@@ -34121,6 +35301,9 @@
       <c r="BD165" t="s">
         <v>4962</v>
       </c>
+      <c r="BE165" t="s">
+        <v>5931</v>
+      </c>
       <c r="BF165" t="s">
         <v>5181</v>
       </c>
@@ -34153,6 +35336,9 @@
       <c r="BD166" t="s">
         <v>4963</v>
       </c>
+      <c r="BE166" t="s">
+        <v>5932</v>
+      </c>
       <c r="BF166" t="s">
         <v>5182</v>
       </c>
@@ -34185,6 +35371,9 @@
       <c r="BD167" t="s">
         <v>4964</v>
       </c>
+      <c r="BE167" t="s">
+        <v>5933</v>
+      </c>
       <c r="BF167" t="s">
         <v>5183</v>
       </c>
@@ -34217,6 +35406,9 @@
       <c r="BD168" t="s">
         <v>4965</v>
       </c>
+      <c r="BE168" t="s">
+        <v>5934</v>
+      </c>
       <c r="BF168" t="s">
         <v>5184</v>
       </c>
@@ -34249,6 +35441,9 @@
       <c r="BD169" t="s">
         <v>4966</v>
       </c>
+      <c r="BE169" t="s">
+        <v>5935</v>
+      </c>
       <c r="BF169" t="s">
         <v>5185</v>
       </c>
@@ -34278,6 +35473,9 @@
       <c r="BD170" t="s">
         <v>4967</v>
       </c>
+      <c r="BE170" t="s">
+        <v>5936</v>
+      </c>
       <c r="BF170" t="s">
         <v>5186</v>
       </c>
@@ -34307,6 +35505,9 @@
       <c r="BD171" t="s">
         <v>4968</v>
       </c>
+      <c r="BE171" t="s">
+        <v>5937</v>
+      </c>
       <c r="BF171" t="s">
         <v>5187</v>
       </c>
@@ -34336,6 +35537,9 @@
       <c r="BD172" t="s">
         <v>4969</v>
       </c>
+      <c r="BE172" t="s">
+        <v>5938</v>
+      </c>
       <c r="BF172" t="s">
         <v>5188</v>
       </c>
@@ -34365,6 +35569,9 @@
       <c r="BD173" t="s">
         <v>4970</v>
       </c>
+      <c r="BE173" t="s">
+        <v>5939</v>
+      </c>
       <c r="BF173" t="s">
         <v>5189</v>
       </c>
@@ -34394,6 +35601,9 @@
       <c r="BD174" t="s">
         <v>4971</v>
       </c>
+      <c r="BE174" t="s">
+        <v>5940</v>
+      </c>
       <c r="BF174" t="s">
         <v>5190</v>
       </c>
@@ -34423,6 +35633,9 @@
       <c r="BD175" t="s">
         <v>4972</v>
       </c>
+      <c r="BE175" t="s">
+        <v>5941</v>
+      </c>
       <c r="BF175" t="s">
         <v>5191</v>
       </c>
@@ -34452,6 +35665,9 @@
       <c r="BD176" t="s">
         <v>4973</v>
       </c>
+      <c r="BE176" t="s">
+        <v>5942</v>
+      </c>
       <c r="BF176" t="s">
         <v>5192</v>
       </c>
@@ -34481,6 +35697,9 @@
       <c r="BD177" t="s">
         <v>4974</v>
       </c>
+      <c r="BE177" t="s">
+        <v>5943</v>
+      </c>
       <c r="BF177" t="s">
         <v>5193</v>
       </c>
@@ -34510,6 +35729,9 @@
       <c r="BD178" t="s">
         <v>4975</v>
       </c>
+      <c r="BE178" t="s">
+        <v>5944</v>
+      </c>
       <c r="BF178" t="s">
         <v>5194</v>
       </c>
@@ -34539,6 +35761,9 @@
       <c r="BD179" t="s">
         <v>4976</v>
       </c>
+      <c r="BE179" t="s">
+        <v>5945</v>
+      </c>
       <c r="BF179" t="s">
         <v>5195</v>
       </c>
@@ -34568,6 +35793,9 @@
       <c r="BD180" t="s">
         <v>4977</v>
       </c>
+      <c r="BE180" t="s">
+        <v>5946</v>
+      </c>
       <c r="BF180" t="s">
         <v>5196</v>
       </c>
@@ -34597,6 +35825,9 @@
       <c r="BD181" t="s">
         <v>4978</v>
       </c>
+      <c r="BE181" t="s">
+        <v>5947</v>
+      </c>
       <c r="BF181" t="s">
         <v>5197</v>
       </c>
@@ -34626,6 +35857,9 @@
       <c r="BD182" t="s">
         <v>4979</v>
       </c>
+      <c r="BE182" t="s">
+        <v>5948</v>
+      </c>
       <c r="BF182" t="s">
         <v>5198</v>
       </c>
@@ -34655,6 +35889,9 @@
       <c r="BD183" t="s">
         <v>4980</v>
       </c>
+      <c r="BE183" t="s">
+        <v>5949</v>
+      </c>
       <c r="BF183" t="s">
         <v>5199</v>
       </c>
@@ -34684,6 +35921,9 @@
       <c r="BD184" t="s">
         <v>4981</v>
       </c>
+      <c r="BE184" t="s">
+        <v>5950</v>
+      </c>
       <c r="BF184" t="s">
         <v>5200</v>
       </c>
@@ -34713,6 +35953,9 @@
       <c r="BD185" t="s">
         <v>4982</v>
       </c>
+      <c r="BE185" t="s">
+        <v>5951</v>
+      </c>
       <c r="BF185" t="s">
         <v>5201</v>
       </c>
@@ -34742,6 +35985,9 @@
       <c r="BD186" t="s">
         <v>4983</v>
       </c>
+      <c r="BE186" t="s">
+        <v>5952</v>
+      </c>
       <c r="BF186" t="s">
         <v>5202</v>
       </c>
@@ -34768,6 +36014,9 @@
       <c r="BD187" t="s">
         <v>4984</v>
       </c>
+      <c r="BE187" t="s">
+        <v>5953</v>
+      </c>
       <c r="BF187" t="s">
         <v>5203</v>
       </c>
@@ -34794,6 +36043,9 @@
       <c r="BD188" t="s">
         <v>4985</v>
       </c>
+      <c r="BE188" t="s">
+        <v>5954</v>
+      </c>
       <c r="BF188" t="s">
         <v>5204</v>
       </c>
@@ -34820,6 +36072,9 @@
       <c r="BD189" t="s">
         <v>4986</v>
       </c>
+      <c r="BE189" t="s">
+        <v>5955</v>
+      </c>
       <c r="BF189" t="s">
         <v>5205</v>
       </c>
@@ -34846,6 +36101,9 @@
       <c r="BD190" t="s">
         <v>4987</v>
       </c>
+      <c r="BE190" t="s">
+        <v>5956</v>
+      </c>
       <c r="BF190" t="s">
         <v>5206</v>
       </c>
@@ -34872,6 +36130,9 @@
       <c r="BD191" t="s">
         <v>4988</v>
       </c>
+      <c r="BE191" t="s">
+        <v>5957</v>
+      </c>
       <c r="BF191" t="s">
         <v>5207</v>
       </c>
@@ -34898,6 +36159,9 @@
       <c r="BD192" t="s">
         <v>4989</v>
       </c>
+      <c r="BE192" t="s">
+        <v>5958</v>
+      </c>
       <c r="BF192" t="s">
         <v>5208</v>
       </c>
@@ -34924,6 +36188,9 @@
       <c r="BD193" t="s">
         <v>4990</v>
       </c>
+      <c r="BE193" t="s">
+        <v>5959</v>
+      </c>
       <c r="BF193" t="s">
         <v>5209</v>
       </c>
@@ -34950,6 +36217,9 @@
       <c r="BD194" t="s">
         <v>4991</v>
       </c>
+      <c r="BE194" t="s">
+        <v>5960</v>
+      </c>
       <c r="BF194" t="s">
         <v>5210</v>
       </c>
@@ -34976,6 +36246,9 @@
       <c r="BD195" t="s">
         <v>4992</v>
       </c>
+      <c r="BE195" t="s">
+        <v>5961</v>
+      </c>
       <c r="BF195" t="s">
         <v>5211</v>
       </c>
@@ -35002,6 +36275,9 @@
       <c r="BD196" t="s">
         <v>4993</v>
       </c>
+      <c r="BE196" t="s">
+        <v>5962</v>
+      </c>
       <c r="BF196" t="s">
         <v>5212</v>
       </c>
@@ -35028,6 +36304,9 @@
       <c r="BD197" t="s">
         <v>4994</v>
       </c>
+      <c r="BE197" t="s">
+        <v>5963</v>
+      </c>
       <c r="BF197" t="s">
         <v>5213</v>
       </c>
@@ -35054,6 +36333,9 @@
       <c r="BD198" t="s">
         <v>4995</v>
       </c>
+      <c r="BE198" t="s">
+        <v>5964</v>
+      </c>
       <c r="BF198" t="s">
         <v>5214</v>
       </c>
@@ -35080,6 +36362,9 @@
       <c r="BD199" t="s">
         <v>4996</v>
       </c>
+      <c r="BE199" t="s">
+        <v>5965</v>
+      </c>
       <c r="BF199" t="s">
         <v>5215</v>
       </c>
@@ -35106,6 +36391,9 @@
       <c r="BD200" t="s">
         <v>4997</v>
       </c>
+      <c r="BE200" t="s">
+        <v>5966</v>
+      </c>
       <c r="BF200" t="s">
         <v>5216</v>
       </c>
@@ -35132,6 +36420,9 @@
       <c r="BD201" t="s">
         <v>4998</v>
       </c>
+      <c r="BE201" t="s">
+        <v>5967</v>
+      </c>
       <c r="BF201" t="s">
         <v>5217</v>
       </c>
@@ -35158,6 +36449,9 @@
       <c r="BD202" t="s">
         <v>4999</v>
       </c>
+      <c r="BE202" t="s">
+        <v>5968</v>
+      </c>
       <c r="BF202" t="s">
         <v>5218</v>
       </c>
@@ -35184,6 +36478,9 @@
       <c r="BD203" t="s">
         <v>5000</v>
       </c>
+      <c r="BE203" t="s">
+        <v>5969</v>
+      </c>
       <c r="BF203" t="s">
         <v>5219</v>
       </c>
@@ -35210,6 +36507,9 @@
       <c r="BD204" t="s">
         <v>5001</v>
       </c>
+      <c r="BE204" t="s">
+        <v>5970</v>
+      </c>
       <c r="BF204" t="s">
         <v>5220</v>
       </c>
@@ -35236,6 +36536,9 @@
       <c r="BD205" t="s">
         <v>5002</v>
       </c>
+      <c r="BE205" t="s">
+        <v>5971</v>
+      </c>
       <c r="BF205" t="s">
         <v>5221</v>
       </c>
@@ -35262,6 +36565,9 @@
       <c r="BD206" t="s">
         <v>5003</v>
       </c>
+      <c r="BE206" t="s">
+        <v>5972</v>
+      </c>
       <c r="BF206" t="s">
         <v>5222</v>
       </c>
@@ -35288,6 +36594,9 @@
       <c r="BD207" t="s">
         <v>5004</v>
       </c>
+      <c r="BE207" t="s">
+        <v>5973</v>
+      </c>
       <c r="BF207" t="s">
         <v>5223</v>
       </c>
@@ -35314,6 +36623,9 @@
       <c r="BD208" t="s">
         <v>5005</v>
       </c>
+      <c r="BE208" t="s">
+        <v>5974</v>
+      </c>
       <c r="BF208" t="s">
         <v>5224</v>
       </c>
@@ -35340,6 +36652,9 @@
       <c r="BD209" t="s">
         <v>5006</v>
       </c>
+      <c r="BE209" t="s">
+        <v>5975</v>
+      </c>
       <c r="BF209" t="s">
         <v>5225</v>
       </c>
@@ -35363,6 +36678,9 @@
       <c r="BD210" t="s">
         <v>5007</v>
       </c>
+      <c r="BE210" t="s">
+        <v>5976</v>
+      </c>
       <c r="BF210" t="s">
         <v>5226</v>
       </c>
@@ -35383,6 +36701,9 @@
       <c r="BD211" t="s">
         <v>5008</v>
       </c>
+      <c r="BE211" t="s">
+        <v>5977</v>
+      </c>
       <c r="BF211" t="s">
         <v>5227</v>
       </c>
@@ -35403,6 +36724,9 @@
       <c r="BD212" t="s">
         <v>5009</v>
       </c>
+      <c r="BE212" t="s">
+        <v>5978</v>
+      </c>
       <c r="BF212" t="s">
         <v>5228</v>
       </c>
@@ -35423,6 +36747,9 @@
       <c r="BD213" t="s">
         <v>5010</v>
       </c>
+      <c r="BE213" t="s">
+        <v>5979</v>
+      </c>
       <c r="BF213" t="s">
         <v>5229</v>
       </c>
@@ -35443,6 +36770,9 @@
       <c r="BD214" t="s">
         <v>5011</v>
       </c>
+      <c r="BE214" t="s">
+        <v>5980</v>
+      </c>
       <c r="BF214" t="s">
         <v>5230</v>
       </c>
@@ -35463,6 +36793,9 @@
       <c r="BD215" t="s">
         <v>5012</v>
       </c>
+      <c r="BE215" t="s">
+        <v>5981</v>
+      </c>
       <c r="BF215" t="s">
         <v>5231</v>
       </c>
@@ -35483,6 +36816,9 @@
       <c r="BD216" t="s">
         <v>5013</v>
       </c>
+      <c r="BE216" t="s">
+        <v>5982</v>
+      </c>
       <c r="BF216" t="s">
         <v>5232</v>
       </c>
@@ -35503,6 +36839,9 @@
       <c r="BD217" t="s">
         <v>5014</v>
       </c>
+      <c r="BE217" t="s">
+        <v>5983</v>
+      </c>
       <c r="BF217" t="s">
         <v>5233</v>
       </c>
@@ -35523,6 +36862,9 @@
       <c r="BD218" t="s">
         <v>5015</v>
       </c>
+      <c r="BE218" t="s">
+        <v>5984</v>
+      </c>
       <c r="BF218" t="s">
         <v>5234</v>
       </c>
@@ -35540,6 +36882,9 @@
       <c r="BD219" t="s">
         <v>5016</v>
       </c>
+      <c r="BE219" t="s">
+        <v>5985</v>
+      </c>
       <c r="BF219" t="s">
         <v>5235</v>
       </c>
@@ -35557,6 +36902,9 @@
       <c r="BD220" t="s">
         <v>5017</v>
       </c>
+      <c r="BE220" t="s">
+        <v>5986</v>
+      </c>
       <c r="BF220" t="s">
         <v>5236</v>
       </c>
@@ -35571,6 +36919,9 @@
       <c r="BB221" t="s">
         <v>4580</v>
       </c>
+      <c r="BE221" t="s">
+        <v>5987</v>
+      </c>
       <c r="BF221" t="s">
         <v>5237</v>
       </c>
@@ -35585,6 +36936,9 @@
       <c r="BB222" t="s">
         <v>4581</v>
       </c>
+      <c r="BE222" t="s">
+        <v>5988</v>
+      </c>
       <c r="BF222" t="s">
         <v>5238</v>
       </c>
@@ -35596,6 +36950,9 @@
       </c>
     </row>
     <row r="223" spans="52:60">
+      <c r="BE223" t="s">
+        <v>5989</v>
+      </c>
       <c r="BF223" t="s">
         <v>5239</v>
       </c>
@@ -35607,6 +36964,9 @@
       </c>
     </row>
     <row r="224" spans="52:60">
+      <c r="BE224" t="s">
+        <v>5990</v>
+      </c>
       <c r="BF224" t="s">
         <v>5240</v>
       </c>
@@ -35617,7 +36977,10 @@
         <v>5721</v>
       </c>
     </row>
-    <row r="225" spans="58:60">
+    <row r="225" spans="57:60">
+      <c r="BE225" t="s">
+        <v>5991</v>
+      </c>
       <c r="BF225" t="s">
         <v>5241</v>
       </c>
@@ -35628,7 +36991,10 @@
         <v>5722</v>
       </c>
     </row>
-    <row r="226" spans="58:60">
+    <row r="226" spans="57:60">
+      <c r="BE226" t="s">
+        <v>5992</v>
+      </c>
       <c r="BF226" t="s">
         <v>5242</v>
       </c>
@@ -35639,7 +37005,10 @@
         <v>5723</v>
       </c>
     </row>
-    <row r="227" spans="58:60">
+    <row r="227" spans="57:60">
+      <c r="BE227" t="s">
+        <v>5993</v>
+      </c>
       <c r="BF227" t="s">
         <v>5243</v>
       </c>
@@ -35650,7 +37019,10 @@
         <v>5724</v>
       </c>
     </row>
-    <row r="228" spans="58:60">
+    <row r="228" spans="57:60">
+      <c r="BE228" t="s">
+        <v>5994</v>
+      </c>
       <c r="BF228" t="s">
         <v>5244</v>
       </c>
@@ -35661,7 +37033,10 @@
         <v>5725</v>
       </c>
     </row>
-    <row r="229" spans="58:60">
+    <row r="229" spans="57:60">
+      <c r="BE229" t="s">
+        <v>5995</v>
+      </c>
       <c r="BF229" t="s">
         <v>5245</v>
       </c>
@@ -35672,7 +37047,10 @@
         <v>5726</v>
       </c>
     </row>
-    <row r="230" spans="58:60">
+    <row r="230" spans="57:60">
+      <c r="BE230" t="s">
+        <v>5996</v>
+      </c>
       <c r="BF230" t="s">
         <v>5246</v>
       </c>
@@ -35683,7 +37061,7 @@
         <v>5727</v>
       </c>
     </row>
-    <row r="231" spans="58:60">
+    <row r="231" spans="57:60">
       <c r="BF231" t="s">
         <v>5247</v>
       </c>
@@ -35694,7 +37072,7 @@
         <v>5728</v>
       </c>
     </row>
-    <row r="232" spans="58:60">
+    <row r="232" spans="57:60">
       <c r="BF232" t="s">
         <v>5248</v>
       </c>
@@ -35705,7 +37083,7 @@
         <v>5729</v>
       </c>
     </row>
-    <row r="233" spans="58:60">
+    <row r="233" spans="57:60">
       <c r="BF233" t="s">
         <v>5249</v>
       </c>
@@ -35716,7 +37094,7 @@
         <v>5730</v>
       </c>
     </row>
-    <row r="234" spans="58:60">
+    <row r="234" spans="57:60">
       <c r="BF234" t="s">
         <v>5250</v>
       </c>
@@ -35727,7 +37105,7 @@
         <v>5731</v>
       </c>
     </row>
-    <row r="235" spans="58:60">
+    <row r="235" spans="57:60">
       <c r="BF235" t="s">
         <v>5251</v>
       </c>
@@ -35735,7 +37113,7 @@
         <v>5732</v>
       </c>
     </row>
-    <row r="236" spans="58:60">
+    <row r="236" spans="57:60">
       <c r="BF236" t="s">
         <v>5252</v>
       </c>
@@ -35743,7 +37121,7 @@
         <v>5733</v>
       </c>
     </row>
-    <row r="237" spans="58:60">
+    <row r="237" spans="57:60">
       <c r="BF237" t="s">
         <v>5253</v>
       </c>
@@ -35751,7 +37129,7 @@
         <v>5734</v>
       </c>
     </row>
-    <row r="238" spans="58:60">
+    <row r="238" spans="57:60">
       <c r="BF238" t="s">
         <v>5254</v>
       </c>
@@ -35759,7 +37137,7 @@
         <v>5735</v>
       </c>
     </row>
-    <row r="239" spans="58:60">
+    <row r="239" spans="57:60">
       <c r="BF239" t="s">
         <v>5255</v>
       </c>
@@ -35767,7 +37145,7 @@
         <v>5736</v>
       </c>
     </row>
-    <row r="240" spans="58:60">
+    <row r="240" spans="57:60">
       <c r="BF240" t="s">
         <v>5256</v>
       </c>

</xml_diff>